<commit_message>
web services for stakeholder test cases added
</commit_message>
<xml_diff>
--- a/tests/Test Cases/web services for stakeholder.xlsx
+++ b/tests/Test Cases/web services for stakeholder.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Stakeholder should enter his/her valid credential like name, designation, organization name, contact number and email</t>
   </si>
   <si>
-    <t>verify that clicking on "Request" button shows success message</t>
-  </si>
-  <si>
     <t>Clicking on "Search" button should show success message</t>
   </si>
   <si>
@@ -65,12 +62,6 @@
     <t>verify that clicking on "Search" button shows searched student is not available if the student information is not valid</t>
   </si>
   <si>
-    <t>verify that stakeholder clicking on "Submit" button sends stakeholder information to the registrar</t>
-  </si>
-  <si>
-    <t>Clicking on "Submit" button should send stakeholder information to the registrar</t>
-  </si>
-  <si>
     <t>verify that stakeholder clicking on link shows student profile with certificate and other information</t>
   </si>
   <si>
@@ -78,6 +69,30 @@
   </si>
   <si>
     <t>Request for verification</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>verify that clicking on "Search" button shows success message</t>
+  </si>
+  <si>
+    <t>verify that stakeholder clicking on "Request" button sends stakeholder information to the registrar</t>
+  </si>
+  <si>
+    <t>Clicking on "Request" button should send stakeholder information to the registrar</t>
+  </si>
+  <si>
+    <t>verify that after clicking "Request" button stakeholder information send to UGC, Register, Program Officer of corresponding department and student</t>
+  </si>
+  <si>
+    <t>After clicking "Request" button stakeholder information should send to UGC, Register, Program Officer of corresponding department and student</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>In student, he/she does not get any message</t>
   </si>
 </sst>
 </file>
@@ -415,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +445,7 @@
     <col min="5" max="5" width="12.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -447,9 +462,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -460,30 +475,39 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -493,31 +517,52 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25"/>
+        <v>20</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>